<commit_message>
Drafting code for ggplots
</commit_message>
<xml_diff>
--- a/samplemicro.xlsx
+++ b/samplemicro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaelyn\Documents\University\University 2020-2021\thesis\MicrobiomeThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEC886C-C9F5-4FBD-93B9-C64121696D43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20592361-3E38-4401-9C8D-2F9AFABAAD02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2295" yWindow="2865" windowWidth="15060" windowHeight="8325" xr2:uid="{10FB8EF1-8FD6-4C4F-8C21-37637CFD308F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="23">
   <si>
     <t>typeOfCoreMicrobiome</t>
   </si>
@@ -98,6 +98,12 @@
   <si>
     <t>p</t>
   </si>
+  <si>
+    <t>common</t>
+  </si>
+  <si>
+    <t>temporal</t>
+  </si>
 </sst>
 </file>
 
@@ -126,7 +132,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -149,16 +155,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -176,6 +197,949 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>sampledata!$F$2:$F$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>common</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>temporal</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ecological</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>functional</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>host-adapted</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>sampledata!$G$2:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BDB9-478A-A42B-C1A6D585CBAB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1220156559"/>
+        <c:axId val="1218861855"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1220156559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="3600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Core Microbiome Type</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="3600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="3600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1218861855"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1218861855"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="3600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Number of Papers </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="3600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="3600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1220156559"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="3600" baseline="0"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1384526</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>595312</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{128D6BAB-B5FE-48C7-9110-6932E81A6587}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -475,10 +1439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA747E64-1B34-418D-9D97-9F20E2B8F5F9}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="W38" sqref="W38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +1453,7 @@
     <col min="4" max="4" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +1467,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -516,8 +1480,14 @@
       <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -528,8 +1498,14 @@
       <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -540,8 +1516,14 @@
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -552,8 +1534,14 @@
       <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -566,8 +1554,14 @@
       <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>4</v>
@@ -579,7 +1573,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>4</v>
@@ -591,7 +1585,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>4</v>
@@ -603,7 +1597,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>4</v>
@@ -615,7 +1609,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -629,7 +1623,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>4</v>
@@ -641,7 +1635,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
         <v>5</v>
@@ -653,7 +1647,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
         <v>4</v>
@@ -665,7 +1659,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
         <v>4</v>
@@ -677,7 +1671,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
         <v>4</v>
@@ -1156,6 +2150,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>